<commit_message>
Adding time tracking sheet button to dev post week 2
</commit_message>
<xml_diff>
--- a/docs/JordanMartin_Week1_TimeTracking.xlsx
+++ b/docs/JordanMartin_Week1_TimeTracking.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucf-my.sharepoint.com/personal/jo309551_ucf_edu/Documents/Spring 2020/Toggl/PPP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Batcave\website\jordantommartin.github.io\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{BD11ED11-32E1-4E6C-BF50-B651A23A2F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{206DE11E-D22D-440F-ADCA-DCA667E81427}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A680BC-EF85-4D5D-8902-D63B60628E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time Sheet" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -663,10 +663,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[h]:mm"/>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <numFmt numFmtId="26" formatCode="h:mm:ss"/>
     </dxf>
@@ -1389,7 +1386,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -1562,7 +1559,7 @@
     <dataField name="Sum of Duration" fld="11" baseField="3" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="6">
+    <format dxfId="5">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -1589,11 +1586,11 @@
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Task"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Description"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Billable"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Start date" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Start time" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="End date" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="End time" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Duration" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Start date" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Start time" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="End date" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="End time" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Duration" dataDxfId="0"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Tags"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Amount ()"/>
   </tableColumns>
@@ -1900,7 +1897,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -2081,8 +2078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N76"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:N34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2368,7 +2365,7 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G8" t="s">
         <v>20</v>
@@ -2403,7 +2400,7 @@
         <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G9" t="s">
         <v>20</v>

</xml_diff>